<commit_message>
update anp shoe model and filledin
</commit_message>
<xml_diff>
--- a/Examples/ANP_Athletic_Shoes/Athletic Shoes model_empty.xlsx
+++ b/Examples/ANP_Athletic_Shoes/Athletic Shoes model_empty.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="24">
   <si>
     <t>Adidas</t>
   </si>
@@ -494,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G420"/>
+  <dimension ref="A1:G429"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2883,22 +2883,22 @@
     </row>
     <row r="204" spans="1:7">
       <c r="A204" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D204" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E204" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F204" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G204" s="4" t="s">
         <v>4</v>
@@ -2906,7 +2906,7 @@
     </row>
     <row r="205" spans="1:7">
       <c r="A205" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B205" s="5">
         <v>1</v>
@@ -2919,7 +2919,7 @@
     </row>
     <row r="206" spans="1:7">
       <c r="A206" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B206" s="8">
         <f>1/C205</f>
@@ -2935,7 +2935,7 @@
     </row>
     <row r="207" spans="1:7">
       <c r="A207" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B207" s="8">
         <f>1/D205</f>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="208" spans="1:7">
       <c r="A208" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B208" s="8">
         <f>1/E205</f>
@@ -2976,7 +2976,7 @@
     </row>
     <row r="209" spans="1:7">
       <c r="A209" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B209" s="8">
         <f>1/F205</f>
@@ -3000,1156 +3000,1156 @@
       <c r="G209" s="7"/>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="1" t="s">
-        <v>10</v>
+      <c r="A212" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="2" t="s">
-        <v>1</v>
+      <c r="A213" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B213" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C213" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D213" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E213" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F213" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G213" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="214" spans="1:7">
-      <c r="A214" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B214" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C214" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D214" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E214" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A214" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B214" s="5">
+        <v>1</v>
+      </c>
+      <c r="C214" s="6"/>
+      <c r="D214" s="6"/>
+      <c r="E214" s="6"/>
+      <c r="F214" s="6"/>
+      <c r="G214" s="7"/>
     </row>
     <row r="215" spans="1:7">
       <c r="A215" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B215" s="5">
-        <v>1</v>
-      </c>
-      <c r="C215" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="B215" s="8">
+        <f>1/C214</f>
+        <v>0</v>
+      </c>
+      <c r="C215" s="5">
+        <v>1</v>
+      </c>
       <c r="D215" s="6"/>
-      <c r="E215" s="7"/>
+      <c r="E215" s="6"/>
+      <c r="F215" s="6"/>
+      <c r="G215" s="7"/>
     </row>
     <row r="216" spans="1:7">
       <c r="A216" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B216" s="8">
-        <f>1/C215</f>
-        <v>0</v>
-      </c>
-      <c r="C216" s="5">
-        <v>1</v>
-      </c>
-      <c r="D216" s="6"/>
-      <c r="E216" s="7"/>
+        <f>1/D214</f>
+        <v>0</v>
+      </c>
+      <c r="C216" s="8">
+        <f>1/D215</f>
+        <v>0</v>
+      </c>
+      <c r="D216" s="5">
+        <v>1</v>
+      </c>
+      <c r="E216" s="6"/>
+      <c r="F216" s="6"/>
+      <c r="G216" s="7"/>
     </row>
     <row r="217" spans="1:7">
       <c r="A217" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B217" s="8">
+        <f>1/E214</f>
+        <v>0</v>
+      </c>
+      <c r="C217" s="8">
+        <f>1/E215</f>
+        <v>0</v>
+      </c>
+      <c r="D217" s="8">
+        <f>1/E216</f>
+        <v>0</v>
+      </c>
+      <c r="E217" s="5">
+        <v>1</v>
+      </c>
+      <c r="F217" s="6"/>
+      <c r="G217" s="7"/>
+    </row>
+    <row r="218" spans="1:7">
+      <c r="A218" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B218" s="8">
+        <f>1/F214</f>
+        <v>0</v>
+      </c>
+      <c r="C218" s="8">
+        <f>1/F215</f>
+        <v>0</v>
+      </c>
+      <c r="D218" s="8">
+        <f>1/F216</f>
+        <v>0</v>
+      </c>
+      <c r="E218" s="8">
+        <f>1/F217</f>
+        <v>0</v>
+      </c>
+      <c r="F218" s="5">
+        <v>1</v>
+      </c>
+      <c r="G218" s="7"/>
+    </row>
+    <row r="221" spans="1:7">
+      <c r="A221" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7">
+      <c r="A222" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7">
+      <c r="A223" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B223" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C223" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D223" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B217" s="8">
-        <f>1/D215</f>
-        <v>0</v>
-      </c>
-      <c r="C217" s="8">
-        <f>1/D216</f>
-        <v>0</v>
-      </c>
-      <c r="D217" s="5">
-        <v>1</v>
-      </c>
-      <c r="E217" s="7"/>
-    </row>
-    <row r="220" spans="1:7">
-      <c r="A220" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="221" spans="1:7">
-      <c r="A221" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B221" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C221" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D221" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E221" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F221" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G221" s="4" t="s">
+      <c r="E223" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="222" spans="1:7">
-      <c r="A222" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B222" s="5">
-        <v>1</v>
-      </c>
-      <c r="C222" s="6"/>
-      <c r="D222" s="6"/>
-      <c r="E222" s="6"/>
-      <c r="F222" s="6"/>
-      <c r="G222" s="7"/>
-    </row>
-    <row r="223" spans="1:7">
-      <c r="A223" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B223" s="8">
-        <f>1/C222</f>
-        <v>0</v>
-      </c>
-      <c r="C223" s="5">
-        <v>1</v>
-      </c>
-      <c r="D223" s="6"/>
-      <c r="E223" s="6"/>
-      <c r="F223" s="6"/>
-      <c r="G223" s="7"/>
     </row>
     <row r="224" spans="1:7">
       <c r="A224" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B224" s="8">
-        <f>1/D222</f>
-        <v>0</v>
-      </c>
-      <c r="C224" s="8">
-        <f>1/D223</f>
-        <v>0</v>
-      </c>
-      <c r="D224" s="5">
-        <v>1</v>
-      </c>
-      <c r="E224" s="6"/>
-      <c r="F224" s="6"/>
-      <c r="G224" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="B224" s="5">
+        <v>1</v>
+      </c>
+      <c r="C224" s="6"/>
+      <c r="D224" s="6"/>
+      <c r="E224" s="7"/>
     </row>
     <row r="225" spans="1:7">
       <c r="A225" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B225" s="8">
-        <f>1/E222</f>
-        <v>0</v>
-      </c>
-      <c r="C225" s="8">
-        <f>1/E223</f>
-        <v>0</v>
-      </c>
-      <c r="D225" s="8">
-        <f>1/E224</f>
-        <v>0</v>
-      </c>
-      <c r="E225" s="5">
-        <v>1</v>
-      </c>
-      <c r="F225" s="6"/>
-      <c r="G225" s="7"/>
+        <f>1/C224</f>
+        <v>0</v>
+      </c>
+      <c r="C225" s="5">
+        <v>1</v>
+      </c>
+      <c r="D225" s="6"/>
+      <c r="E225" s="7"/>
     </row>
     <row r="226" spans="1:7">
       <c r="A226" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B226" s="8">
+        <f>1/D224</f>
+        <v>0</v>
+      </c>
+      <c r="C226" s="8">
+        <f>1/D225</f>
+        <v>0</v>
+      </c>
+      <c r="D226" s="5">
+        <v>1</v>
+      </c>
+      <c r="E226" s="7"/>
+    </row>
+    <row r="229" spans="1:7">
+      <c r="A229" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7">
+      <c r="A230" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B230" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C230" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D230" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E230" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F230" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B226" s="8">
-        <f>1/F222</f>
-        <v>0</v>
-      </c>
-      <c r="C226" s="8">
-        <f>1/F223</f>
-        <v>0</v>
-      </c>
-      <c r="D226" s="8">
-        <f>1/F224</f>
-        <v>0</v>
-      </c>
-      <c r="E226" s="8">
-        <f>1/F225</f>
-        <v>0</v>
-      </c>
-      <c r="F226" s="5">
-        <v>1</v>
-      </c>
-      <c r="G226" s="7"/>
-    </row>
-    <row r="229" spans="1:7">
-      <c r="A229" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="230" spans="1:7">
-      <c r="A230" s="2" t="s">
-        <v>1</v>
+      <c r="G230" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="231" spans="1:7">
-      <c r="A231" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B231" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C231" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D231" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E231" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A231" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B231" s="5">
+        <v>1</v>
+      </c>
+      <c r="C231" s="6"/>
+      <c r="D231" s="6"/>
+      <c r="E231" s="6"/>
+      <c r="F231" s="6"/>
+      <c r="G231" s="7"/>
     </row>
     <row r="232" spans="1:7">
       <c r="A232" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B232" s="5">
-        <v>1</v>
-      </c>
-      <c r="C232" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="B232" s="8">
+        <f>1/C231</f>
+        <v>0</v>
+      </c>
+      <c r="C232" s="5">
+        <v>1</v>
+      </c>
       <c r="D232" s="6"/>
-      <c r="E232" s="7"/>
+      <c r="E232" s="6"/>
+      <c r="F232" s="6"/>
+      <c r="G232" s="7"/>
     </row>
     <row r="233" spans="1:7">
       <c r="A233" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B233" s="8">
-        <f>1/C232</f>
-        <v>0</v>
-      </c>
-      <c r="C233" s="5">
-        <v>1</v>
-      </c>
-      <c r="D233" s="6"/>
-      <c r="E233" s="7"/>
+        <f>1/D231</f>
+        <v>0</v>
+      </c>
+      <c r="C233" s="8">
+        <f>1/D232</f>
+        <v>0</v>
+      </c>
+      <c r="D233" s="5">
+        <v>1</v>
+      </c>
+      <c r="E233" s="6"/>
+      <c r="F233" s="6"/>
+      <c r="G233" s="7"/>
     </row>
     <row r="234" spans="1:7">
       <c r="A234" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B234" s="8">
+        <f>1/E231</f>
+        <v>0</v>
+      </c>
+      <c r="C234" s="8">
+        <f>1/E232</f>
+        <v>0</v>
+      </c>
+      <c r="D234" s="8">
+        <f>1/E233</f>
+        <v>0</v>
+      </c>
+      <c r="E234" s="5">
+        <v>1</v>
+      </c>
+      <c r="F234" s="6"/>
+      <c r="G234" s="7"/>
+    </row>
+    <row r="235" spans="1:7">
+      <c r="A235" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B235" s="8">
+        <f>1/F231</f>
+        <v>0</v>
+      </c>
+      <c r="C235" s="8">
+        <f>1/F232</f>
+        <v>0</v>
+      </c>
+      <c r="D235" s="8">
+        <f>1/F233</f>
+        <v>0</v>
+      </c>
+      <c r="E235" s="8">
+        <f>1/F234</f>
+        <v>0</v>
+      </c>
+      <c r="F235" s="5">
+        <v>1</v>
+      </c>
+      <c r="G235" s="7"/>
+    </row>
+    <row r="238" spans="1:7">
+      <c r="A238" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7">
+      <c r="A239" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7">
+      <c r="A240" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B240" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C240" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D240" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B234" s="8">
-        <f>1/D232</f>
-        <v>0</v>
-      </c>
-      <c r="C234" s="8">
-        <f>1/D233</f>
-        <v>0</v>
-      </c>
-      <c r="D234" s="5">
-        <v>1</v>
-      </c>
-      <c r="E234" s="7"/>
-    </row>
-    <row r="237" spans="1:7">
-      <c r="A237" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="238" spans="1:7">
-      <c r="A238" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B238" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C238" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D238" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E238" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F238" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G238" s="4" t="s">
+      <c r="E240" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="239" spans="1:7">
-      <c r="A239" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B239" s="5">
-        <v>1</v>
-      </c>
-      <c r="C239" s="6"/>
-      <c r="D239" s="6"/>
-      <c r="E239" s="6"/>
-      <c r="F239" s="6"/>
-      <c r="G239" s="7"/>
-    </row>
-    <row r="240" spans="1:7">
-      <c r="A240" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B240" s="8">
-        <f>1/C239</f>
-        <v>0</v>
-      </c>
-      <c r="C240" s="5">
-        <v>1</v>
-      </c>
-      <c r="D240" s="6"/>
-      <c r="E240" s="6"/>
-      <c r="F240" s="6"/>
-      <c r="G240" s="7"/>
     </row>
     <row r="241" spans="1:7">
       <c r="A241" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B241" s="8">
-        <f>1/D239</f>
-        <v>0</v>
-      </c>
-      <c r="C241" s="8">
-        <f>1/D240</f>
-        <v>0</v>
-      </c>
-      <c r="D241" s="5">
-        <v>1</v>
-      </c>
-      <c r="E241" s="6"/>
-      <c r="F241" s="6"/>
-      <c r="G241" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="B241" s="5">
+        <v>1</v>
+      </c>
+      <c r="C241" s="6"/>
+      <c r="D241" s="6"/>
+      <c r="E241" s="7"/>
     </row>
     <row r="242" spans="1:7">
       <c r="A242" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B242" s="8">
-        <f>1/E239</f>
-        <v>0</v>
-      </c>
-      <c r="C242" s="8">
-        <f>1/E240</f>
-        <v>0</v>
-      </c>
-      <c r="D242" s="8">
-        <f>1/E241</f>
-        <v>0</v>
-      </c>
-      <c r="E242" s="5">
-        <v>1</v>
-      </c>
-      <c r="F242" s="6"/>
-      <c r="G242" s="7"/>
+        <f>1/C241</f>
+        <v>0</v>
+      </c>
+      <c r="C242" s="5">
+        <v>1</v>
+      </c>
+      <c r="D242" s="6"/>
+      <c r="E242" s="7"/>
     </row>
     <row r="243" spans="1:7">
       <c r="A243" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B243" s="8">
+        <f>1/D241</f>
+        <v>0</v>
+      </c>
+      <c r="C243" s="8">
+        <f>1/D242</f>
+        <v>0</v>
+      </c>
+      <c r="D243" s="5">
+        <v>1</v>
+      </c>
+      <c r="E243" s="7"/>
+    </row>
+    <row r="246" spans="1:7">
+      <c r="A246" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7">
+      <c r="A247" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B247" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C247" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D247" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E247" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F247" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B243" s="8">
-        <f>1/F239</f>
-        <v>0</v>
-      </c>
-      <c r="C243" s="8">
-        <f>1/F240</f>
-        <v>0</v>
-      </c>
-      <c r="D243" s="8">
-        <f>1/F241</f>
-        <v>0</v>
-      </c>
-      <c r="E243" s="8">
-        <f>1/F242</f>
-        <v>0</v>
-      </c>
-      <c r="F243" s="5">
-        <v>1</v>
-      </c>
-      <c r="G243" s="7"/>
-    </row>
-    <row r="246" spans="1:7">
-      <c r="A246" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="247" spans="1:7">
-      <c r="A247" s="2" t="s">
-        <v>1</v>
+      <c r="G247" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="248" spans="1:7">
-      <c r="A248" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B248" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C248" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D248" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E248" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A248" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B248" s="5">
+        <v>1</v>
+      </c>
+      <c r="C248" s="6"/>
+      <c r="D248" s="6"/>
+      <c r="E248" s="6"/>
+      <c r="F248" s="6"/>
+      <c r="G248" s="7"/>
     </row>
     <row r="249" spans="1:7">
       <c r="A249" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B249" s="5">
-        <v>1</v>
-      </c>
-      <c r="C249" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="B249" s="8">
+        <f>1/C248</f>
+        <v>0</v>
+      </c>
+      <c r="C249" s="5">
+        <v>1</v>
+      </c>
       <c r="D249" s="6"/>
-      <c r="E249" s="7"/>
+      <c r="E249" s="6"/>
+      <c r="F249" s="6"/>
+      <c r="G249" s="7"/>
     </row>
     <row r="250" spans="1:7">
       <c r="A250" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B250" s="8">
-        <f>1/C249</f>
-        <v>0</v>
-      </c>
-      <c r="C250" s="5">
-        <v>1</v>
-      </c>
-      <c r="D250" s="6"/>
-      <c r="E250" s="7"/>
+        <f>1/D248</f>
+        <v>0</v>
+      </c>
+      <c r="C250" s="8">
+        <f>1/D249</f>
+        <v>0</v>
+      </c>
+      <c r="D250" s="5">
+        <v>1</v>
+      </c>
+      <c r="E250" s="6"/>
+      <c r="F250" s="6"/>
+      <c r="G250" s="7"/>
     </row>
     <row r="251" spans="1:7">
       <c r="A251" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B251" s="8">
+        <f>1/E248</f>
+        <v>0</v>
+      </c>
+      <c r="C251" s="8">
+        <f>1/E249</f>
+        <v>0</v>
+      </c>
+      <c r="D251" s="8">
+        <f>1/E250</f>
+        <v>0</v>
+      </c>
+      <c r="E251" s="5">
+        <v>1</v>
+      </c>
+      <c r="F251" s="6"/>
+      <c r="G251" s="7"/>
+    </row>
+    <row r="252" spans="1:7">
+      <c r="A252" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B252" s="8">
+        <f>1/F248</f>
+        <v>0</v>
+      </c>
+      <c r="C252" s="8">
+        <f>1/F249</f>
+        <v>0</v>
+      </c>
+      <c r="D252" s="8">
+        <f>1/F250</f>
+        <v>0</v>
+      </c>
+      <c r="E252" s="8">
+        <f>1/F251</f>
+        <v>0</v>
+      </c>
+      <c r="F252" s="5">
+        <v>1</v>
+      </c>
+      <c r="G252" s="7"/>
+    </row>
+    <row r="255" spans="1:7">
+      <c r="A255" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7">
+      <c r="A256" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7">
+      <c r="A257" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B257" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C257" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D257" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B251" s="8">
-        <f>1/D249</f>
-        <v>0</v>
-      </c>
-      <c r="C251" s="8">
-        <f>1/D250</f>
-        <v>0</v>
-      </c>
-      <c r="D251" s="5">
-        <v>1</v>
-      </c>
-      <c r="E251" s="7"/>
-    </row>
-    <row r="254" spans="1:7">
-      <c r="A254" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="255" spans="1:7">
-      <c r="A255" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B255" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C255" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D255" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E255" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F255" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G255" s="4" t="s">
+      <c r="E257" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="256" spans="1:7">
-      <c r="A256" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B256" s="5">
-        <v>1</v>
-      </c>
-      <c r="C256" s="6"/>
-      <c r="D256" s="6"/>
-      <c r="E256" s="6"/>
-      <c r="F256" s="6"/>
-      <c r="G256" s="7"/>
-    </row>
-    <row r="257" spans="1:7">
-      <c r="A257" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B257" s="8">
-        <f>1/C256</f>
-        <v>0</v>
-      </c>
-      <c r="C257" s="5">
-        <v>1</v>
-      </c>
-      <c r="D257" s="6"/>
-      <c r="E257" s="6"/>
-      <c r="F257" s="6"/>
-      <c r="G257" s="7"/>
     </row>
     <row r="258" spans="1:7">
       <c r="A258" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B258" s="8">
-        <f>1/D256</f>
-        <v>0</v>
-      </c>
-      <c r="C258" s="8">
-        <f>1/D257</f>
-        <v>0</v>
-      </c>
-      <c r="D258" s="5">
-        <v>1</v>
-      </c>
-      <c r="E258" s="6"/>
-      <c r="F258" s="6"/>
-      <c r="G258" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="B258" s="5">
+        <v>1</v>
+      </c>
+      <c r="C258" s="6"/>
+      <c r="D258" s="6"/>
+      <c r="E258" s="7"/>
     </row>
     <row r="259" spans="1:7">
       <c r="A259" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B259" s="8">
-        <f>1/E256</f>
-        <v>0</v>
-      </c>
-      <c r="C259" s="8">
-        <f>1/E257</f>
-        <v>0</v>
-      </c>
-      <c r="D259" s="8">
-        <f>1/E258</f>
-        <v>0</v>
-      </c>
-      <c r="E259" s="5">
-        <v>1</v>
-      </c>
-      <c r="F259" s="6"/>
-      <c r="G259" s="7"/>
+        <f>1/C258</f>
+        <v>0</v>
+      </c>
+      <c r="C259" s="5">
+        <v>1</v>
+      </c>
+      <c r="D259" s="6"/>
+      <c r="E259" s="7"/>
     </row>
     <row r="260" spans="1:7">
       <c r="A260" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B260" s="8">
+        <f>1/D258</f>
+        <v>0</v>
+      </c>
+      <c r="C260" s="8">
+        <f>1/D259</f>
+        <v>0</v>
+      </c>
+      <c r="D260" s="5">
+        <v>1</v>
+      </c>
+      <c r="E260" s="7"/>
+    </row>
+    <row r="263" spans="1:7">
+      <c r="A263" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7">
+      <c r="A264" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B264" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C264" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D264" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E264" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F264" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B260" s="8">
-        <f>1/F256</f>
-        <v>0</v>
-      </c>
-      <c r="C260" s="8">
-        <f>1/F257</f>
-        <v>0</v>
-      </c>
-      <c r="D260" s="8">
-        <f>1/F258</f>
-        <v>0</v>
-      </c>
-      <c r="E260" s="8">
-        <f>1/F259</f>
-        <v>0</v>
-      </c>
-      <c r="F260" s="5">
-        <v>1</v>
-      </c>
-      <c r="G260" s="7"/>
-    </row>
-    <row r="263" spans="1:7">
-      <c r="A263" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="264" spans="1:7">
-      <c r="A264" s="2" t="s">
-        <v>1</v>
+      <c r="G264" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="265" spans="1:7">
-      <c r="A265" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B265" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C265" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D265" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E265" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A265" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B265" s="5">
+        <v>1</v>
+      </c>
+      <c r="C265" s="6"/>
+      <c r="D265" s="6"/>
+      <c r="E265" s="6"/>
+      <c r="F265" s="6"/>
+      <c r="G265" s="7"/>
     </row>
     <row r="266" spans="1:7">
       <c r="A266" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B266" s="5">
-        <v>1</v>
-      </c>
-      <c r="C266" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="B266" s="8">
+        <f>1/C265</f>
+        <v>0</v>
+      </c>
+      <c r="C266" s="5">
+        <v>1</v>
+      </c>
       <c r="D266" s="6"/>
-      <c r="E266" s="7"/>
+      <c r="E266" s="6"/>
+      <c r="F266" s="6"/>
+      <c r="G266" s="7"/>
     </row>
     <row r="267" spans="1:7">
       <c r="A267" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B267" s="8">
-        <f>1/C266</f>
-        <v>0</v>
-      </c>
-      <c r="C267" s="5">
-        <v>1</v>
-      </c>
-      <c r="D267" s="6"/>
-      <c r="E267" s="7"/>
+        <f>1/D265</f>
+        <v>0</v>
+      </c>
+      <c r="C267" s="8">
+        <f>1/D266</f>
+        <v>0</v>
+      </c>
+      <c r="D267" s="5">
+        <v>1</v>
+      </c>
+      <c r="E267" s="6"/>
+      <c r="F267" s="6"/>
+      <c r="G267" s="7"/>
     </row>
     <row r="268" spans="1:7">
       <c r="A268" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B268" s="8">
+        <f>1/E265</f>
+        <v>0</v>
+      </c>
+      <c r="C268" s="8">
+        <f>1/E266</f>
+        <v>0</v>
+      </c>
+      <c r="D268" s="8">
+        <f>1/E267</f>
+        <v>0</v>
+      </c>
+      <c r="E268" s="5">
+        <v>1</v>
+      </c>
+      <c r="F268" s="6"/>
+      <c r="G268" s="7"/>
+    </row>
+    <row r="269" spans="1:7">
+      <c r="A269" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B269" s="8">
+        <f>1/F265</f>
+        <v>0</v>
+      </c>
+      <c r="C269" s="8">
+        <f>1/F266</f>
+        <v>0</v>
+      </c>
+      <c r="D269" s="8">
+        <f>1/F267</f>
+        <v>0</v>
+      </c>
+      <c r="E269" s="8">
+        <f>1/F268</f>
+        <v>0</v>
+      </c>
+      <c r="F269" s="5">
+        <v>1</v>
+      </c>
+      <c r="G269" s="7"/>
+    </row>
+    <row r="272" spans="1:7">
+      <c r="A272" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7">
+      <c r="A273" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7">
+      <c r="A274" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B274" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C274" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D274" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B268" s="8">
-        <f>1/D266</f>
-        <v>0</v>
-      </c>
-      <c r="C268" s="8">
-        <f>1/D267</f>
-        <v>0</v>
-      </c>
-      <c r="D268" s="5">
-        <v>1</v>
-      </c>
-      <c r="E268" s="7"/>
-    </row>
-    <row r="271" spans="1:7">
-      <c r="A271" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="272" spans="1:7">
-      <c r="A272" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B272" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C272" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D272" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E272" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F272" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G272" s="4" t="s">
+      <c r="E274" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="273" spans="1:7">
-      <c r="A273" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B273" s="5">
-        <v>1</v>
-      </c>
-      <c r="C273" s="6"/>
-      <c r="D273" s="6"/>
-      <c r="E273" s="6"/>
-      <c r="F273" s="6"/>
-      <c r="G273" s="7"/>
-    </row>
-    <row r="274" spans="1:7">
-      <c r="A274" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B274" s="8">
-        <f>1/C273</f>
-        <v>0</v>
-      </c>
-      <c r="C274" s="5">
-        <v>1</v>
-      </c>
-      <c r="D274" s="6"/>
-      <c r="E274" s="6"/>
-      <c r="F274" s="6"/>
-      <c r="G274" s="7"/>
     </row>
     <row r="275" spans="1:7">
       <c r="A275" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B275" s="8">
-        <f>1/D273</f>
-        <v>0</v>
-      </c>
-      <c r="C275" s="8">
-        <f>1/D274</f>
-        <v>0</v>
-      </c>
-      <c r="D275" s="5">
-        <v>1</v>
-      </c>
-      <c r="E275" s="6"/>
-      <c r="F275" s="6"/>
-      <c r="G275" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="B275" s="5">
+        <v>1</v>
+      </c>
+      <c r="C275" s="6"/>
+      <c r="D275" s="6"/>
+      <c r="E275" s="7"/>
     </row>
     <row r="276" spans="1:7">
       <c r="A276" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B276" s="8">
-        <f>1/E273</f>
-        <v>0</v>
-      </c>
-      <c r="C276" s="8">
-        <f>1/E274</f>
-        <v>0</v>
-      </c>
-      <c r="D276" s="8">
-        <f>1/E275</f>
-        <v>0</v>
-      </c>
-      <c r="E276" s="5">
-        <v>1</v>
-      </c>
-      <c r="F276" s="6"/>
-      <c r="G276" s="7"/>
+        <f>1/C275</f>
+        <v>0</v>
+      </c>
+      <c r="C276" s="5">
+        <v>1</v>
+      </c>
+      <c r="D276" s="6"/>
+      <c r="E276" s="7"/>
     </row>
     <row r="277" spans="1:7">
       <c r="A277" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B277" s="8">
+        <f>1/D275</f>
+        <v>0</v>
+      </c>
+      <c r="C277" s="8">
+        <f>1/D276</f>
+        <v>0</v>
+      </c>
+      <c r="D277" s="5">
+        <v>1</v>
+      </c>
+      <c r="E277" s="7"/>
+    </row>
+    <row r="280" spans="1:7">
+      <c r="A280" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7">
+      <c r="A281" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B281" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C281" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D281" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E281" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F281" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B277" s="8">
-        <f>1/F273</f>
-        <v>0</v>
-      </c>
-      <c r="C277" s="8">
-        <f>1/F274</f>
-        <v>0</v>
-      </c>
-      <c r="D277" s="8">
-        <f>1/F275</f>
-        <v>0</v>
-      </c>
-      <c r="E277" s="8">
-        <f>1/F276</f>
-        <v>0</v>
-      </c>
-      <c r="F277" s="5">
-        <v>1</v>
-      </c>
-      <c r="G277" s="7"/>
-    </row>
-    <row r="280" spans="1:7">
-      <c r="A280" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="281" spans="1:7">
-      <c r="A281" s="2" t="s">
-        <v>1</v>
+      <c r="G281" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="282" spans="1:7">
-      <c r="A282" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B282" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C282" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D282" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E282" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A282" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B282" s="5">
+        <v>1</v>
+      </c>
+      <c r="C282" s="6"/>
+      <c r="D282" s="6"/>
+      <c r="E282" s="6"/>
+      <c r="F282" s="6"/>
+      <c r="G282" s="7"/>
     </row>
     <row r="283" spans="1:7">
       <c r="A283" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B283" s="5">
-        <v>1</v>
-      </c>
-      <c r="C283" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="B283" s="8">
+        <f>1/C282</f>
+        <v>0</v>
+      </c>
+      <c r="C283" s="5">
+        <v>1</v>
+      </c>
       <c r="D283" s="6"/>
-      <c r="E283" s="7"/>
+      <c r="E283" s="6"/>
+      <c r="F283" s="6"/>
+      <c r="G283" s="7"/>
     </row>
     <row r="284" spans="1:7">
       <c r="A284" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B284" s="8">
-        <f>1/C283</f>
-        <v>0</v>
-      </c>
-      <c r="C284" s="5">
-        <v>1</v>
-      </c>
-      <c r="D284" s="6"/>
-      <c r="E284" s="7"/>
+        <f>1/D282</f>
+        <v>0</v>
+      </c>
+      <c r="C284" s="8">
+        <f>1/D283</f>
+        <v>0</v>
+      </c>
+      <c r="D284" s="5">
+        <v>1</v>
+      </c>
+      <c r="E284" s="6"/>
+      <c r="F284" s="6"/>
+      <c r="G284" s="7"/>
     </row>
     <row r="285" spans="1:7">
       <c r="A285" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B285" s="8">
+        <f>1/E282</f>
+        <v>0</v>
+      </c>
+      <c r="C285" s="8">
+        <f>1/E283</f>
+        <v>0</v>
+      </c>
+      <c r="D285" s="8">
+        <f>1/E284</f>
+        <v>0</v>
+      </c>
+      <c r="E285" s="5">
+        <v>1</v>
+      </c>
+      <c r="F285" s="6"/>
+      <c r="G285" s="7"/>
+    </row>
+    <row r="286" spans="1:7">
+      <c r="A286" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B286" s="8">
+        <f>1/F282</f>
+        <v>0</v>
+      </c>
+      <c r="C286" s="8">
+        <f>1/F283</f>
+        <v>0</v>
+      </c>
+      <c r="D286" s="8">
+        <f>1/F284</f>
+        <v>0</v>
+      </c>
+      <c r="E286" s="8">
+        <f>1/F285</f>
+        <v>0</v>
+      </c>
+      <c r="F286" s="5">
+        <v>1</v>
+      </c>
+      <c r="G286" s="7"/>
+    </row>
+    <row r="289" spans="1:7">
+      <c r="A289" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7">
+      <c r="A290" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7">
+      <c r="A291" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B291" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C291" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D291" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B285" s="8">
-        <f>1/D283</f>
-        <v>0</v>
-      </c>
-      <c r="C285" s="8">
-        <f>1/D284</f>
-        <v>0</v>
-      </c>
-      <c r="D285" s="5">
-        <v>1</v>
-      </c>
-      <c r="E285" s="7"/>
-    </row>
-    <row r="288" spans="1:7">
-      <c r="A288" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="289" spans="1:7">
-      <c r="A289" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B289" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C289" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D289" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E289" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F289" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G289" s="4" t="s">
+      <c r="E291" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="290" spans="1:7">
-      <c r="A290" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B290" s="5">
-        <v>1</v>
-      </c>
-      <c r="C290" s="6"/>
-      <c r="D290" s="6"/>
-      <c r="E290" s="6"/>
-      <c r="F290" s="6"/>
-      <c r="G290" s="7"/>
-    </row>
-    <row r="291" spans="1:7">
-      <c r="A291" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B291" s="8">
-        <f>1/C290</f>
-        <v>0</v>
-      </c>
-      <c r="C291" s="5">
-        <v>1</v>
-      </c>
-      <c r="D291" s="6"/>
-      <c r="E291" s="6"/>
-      <c r="F291" s="6"/>
-      <c r="G291" s="7"/>
     </row>
     <row r="292" spans="1:7">
       <c r="A292" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B292" s="8">
-        <f>1/D290</f>
-        <v>0</v>
-      </c>
-      <c r="C292" s="8">
-        <f>1/D291</f>
-        <v>0</v>
-      </c>
-      <c r="D292" s="5">
-        <v>1</v>
-      </c>
-      <c r="E292" s="6"/>
-      <c r="F292" s="6"/>
-      <c r="G292" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="B292" s="5">
+        <v>1</v>
+      </c>
+      <c r="C292" s="6"/>
+      <c r="D292" s="6"/>
+      <c r="E292" s="7"/>
     </row>
     <row r="293" spans="1:7">
       <c r="A293" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B293" s="8">
-        <f>1/E290</f>
-        <v>0</v>
-      </c>
-      <c r="C293" s="8">
-        <f>1/E291</f>
-        <v>0</v>
-      </c>
-      <c r="D293" s="8">
-        <f>1/E292</f>
-        <v>0</v>
-      </c>
-      <c r="E293" s="5">
-        <v>1</v>
-      </c>
-      <c r="F293" s="6"/>
-      <c r="G293" s="7"/>
+        <f>1/C292</f>
+        <v>0</v>
+      </c>
+      <c r="C293" s="5">
+        <v>1</v>
+      </c>
+      <c r="D293" s="6"/>
+      <c r="E293" s="7"/>
     </row>
     <row r="294" spans="1:7">
       <c r="A294" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B294" s="8">
+        <f>1/D292</f>
+        <v>0</v>
+      </c>
+      <c r="C294" s="8">
+        <f>1/D293</f>
+        <v>0</v>
+      </c>
+      <c r="D294" s="5">
+        <v>1</v>
+      </c>
+      <c r="E294" s="7"/>
+    </row>
+    <row r="297" spans="1:7">
+      <c r="A297" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7">
+      <c r="A298" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B298" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C298" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D298" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E298" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F298" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B294" s="8">
-        <f>1/F290</f>
-        <v>0</v>
-      </c>
-      <c r="C294" s="8">
-        <f>1/F291</f>
-        <v>0</v>
-      </c>
-      <c r="D294" s="8">
-        <f>1/F292</f>
-        <v>0</v>
-      </c>
-      <c r="E294" s="8">
-        <f>1/F293</f>
-        <v>0</v>
-      </c>
-      <c r="F294" s="5">
-        <v>1</v>
-      </c>
-      <c r="G294" s="7"/>
-    </row>
-    <row r="297" spans="1:7">
-      <c r="A297" s="1" t="s">
+      <c r="G298" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7">
+      <c r="A299" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="298" spans="1:7">
-      <c r="A298" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="299" spans="1:7">
-      <c r="A299" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B299" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C299" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D299" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E299" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="B299" s="5">
+        <v>1</v>
+      </c>
+      <c r="C299" s="6"/>
+      <c r="D299" s="6"/>
+      <c r="E299" s="6"/>
+      <c r="F299" s="6"/>
+      <c r="G299" s="7"/>
     </row>
     <row r="300" spans="1:7">
       <c r="A300" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B300" s="5">
-        <v>1</v>
-      </c>
-      <c r="C300" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="B300" s="8">
+        <f>1/C299</f>
+        <v>0</v>
+      </c>
+      <c r="C300" s="5">
+        <v>1</v>
+      </c>
       <c r="D300" s="6"/>
-      <c r="E300" s="7"/>
+      <c r="E300" s="6"/>
+      <c r="F300" s="6"/>
+      <c r="G300" s="7"/>
     </row>
     <row r="301" spans="1:7">
       <c r="A301" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B301" s="8">
-        <f>1/C300</f>
-        <v>0</v>
-      </c>
-      <c r="C301" s="5">
-        <v>1</v>
-      </c>
-      <c r="D301" s="6"/>
-      <c r="E301" s="7"/>
+        <f>1/D299</f>
+        <v>0</v>
+      </c>
+      <c r="C301" s="8">
+        <f>1/D300</f>
+        <v>0</v>
+      </c>
+      <c r="D301" s="5">
+        <v>1</v>
+      </c>
+      <c r="E301" s="6"/>
+      <c r="F301" s="6"/>
+      <c r="G301" s="7"/>
     </row>
     <row r="302" spans="1:7">
       <c r="A302" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B302" s="8">
+        <f>1/E299</f>
+        <v>0</v>
+      </c>
+      <c r="C302" s="8">
+        <f>1/E300</f>
+        <v>0</v>
+      </c>
+      <c r="D302" s="8">
+        <f>1/E301</f>
+        <v>0</v>
+      </c>
+      <c r="E302" s="5">
+        <v>1</v>
+      </c>
+      <c r="F302" s="6"/>
+      <c r="G302" s="7"/>
+    </row>
+    <row r="303" spans="1:7">
+      <c r="A303" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B303" s="8">
+        <f>1/F299</f>
+        <v>0</v>
+      </c>
+      <c r="C303" s="8">
+        <f>1/F300</f>
+        <v>0</v>
+      </c>
+      <c r="D303" s="8">
+        <f>1/F301</f>
+        <v>0</v>
+      </c>
+      <c r="E303" s="8">
+        <f>1/F302</f>
+        <v>0</v>
+      </c>
+      <c r="F303" s="5">
+        <v>1</v>
+      </c>
+      <c r="G303" s="7"/>
+    </row>
+    <row r="306" spans="1:7">
+      <c r="A306" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7">
+      <c r="A307" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7">
+      <c r="A308" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B308" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C308" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D308" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B302" s="8">
-        <f>1/D300</f>
-        <v>0</v>
-      </c>
-      <c r="C302" s="8">
-        <f>1/D301</f>
-        <v>0</v>
-      </c>
-      <c r="D302" s="5">
-        <v>1</v>
-      </c>
-      <c r="E302" s="7"/>
-    </row>
-    <row r="305" spans="1:7">
-      <c r="A305" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="306" spans="1:7">
-      <c r="A306" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B306" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C306" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D306" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E306" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F306" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G306" s="4" t="s">
+      <c r="E308" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="307" spans="1:7">
-      <c r="A307" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B307" s="5">
-        <v>1</v>
-      </c>
-      <c r="C307" s="6"/>
-      <c r="D307" s="6"/>
-      <c r="E307" s="6"/>
-      <c r="F307" s="6"/>
-      <c r="G307" s="7"/>
-    </row>
-    <row r="308" spans="1:7">
-      <c r="A308" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B308" s="8">
-        <f>1/C307</f>
-        <v>0</v>
-      </c>
-      <c r="C308" s="5">
-        <v>1</v>
-      </c>
-      <c r="D308" s="6"/>
-      <c r="E308" s="6"/>
-      <c r="F308" s="6"/>
-      <c r="G308" s="7"/>
     </row>
     <row r="309" spans="1:7">
       <c r="A309" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B309" s="8">
-        <f>1/D307</f>
-        <v>0</v>
-      </c>
-      <c r="C309" s="8">
-        <f>1/D308</f>
-        <v>0</v>
-      </c>
-      <c r="D309" s="5">
-        <v>1</v>
-      </c>
-      <c r="E309" s="6"/>
-      <c r="F309" s="6"/>
-      <c r="G309" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="B309" s="5">
+        <v>1</v>
+      </c>
+      <c r="C309" s="6"/>
+      <c r="D309" s="6"/>
+      <c r="E309" s="7"/>
     </row>
     <row r="310" spans="1:7">
       <c r="A310" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B310" s="8">
-        <f>1/E307</f>
-        <v>0</v>
-      </c>
-      <c r="C310" s="8">
-        <f>1/E308</f>
-        <v>0</v>
-      </c>
-      <c r="D310" s="8">
-        <f>1/E309</f>
-        <v>0</v>
-      </c>
-      <c r="E310" s="5">
-        <v>1</v>
-      </c>
-      <c r="F310" s="6"/>
-      <c r="G310" s="7"/>
+        <f>1/C309</f>
+        <v>0</v>
+      </c>
+      <c r="C310" s="5">
+        <v>1</v>
+      </c>
+      <c r="D310" s="6"/>
+      <c r="E310" s="7"/>
     </row>
     <row r="311" spans="1:7">
       <c r="A311" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B311" s="8">
-        <f>1/F307</f>
+        <f>1/D309</f>
         <v>0</v>
       </c>
       <c r="C311" s="8">
-        <f>1/F308</f>
-        <v>0</v>
-      </c>
-      <c r="D311" s="8">
-        <f>1/F309</f>
-        <v>0</v>
-      </c>
-      <c r="E311" s="8">
-        <f>1/F310</f>
-        <v>0</v>
-      </c>
-      <c r="F311" s="5">
-        <v>1</v>
-      </c>
-      <c r="G311" s="7"/>
+        <f>1/D310</f>
+        <v>0</v>
+      </c>
+      <c r="D311" s="5">
+        <v>1</v>
+      </c>
+      <c r="E311" s="7"/>
     </row>
     <row r="314" spans="1:7">
       <c r="A314" s="2" t="s">
@@ -4158,22 +4158,22 @@
     </row>
     <row r="315" spans="1:7">
       <c r="A315" s="3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B315" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C315" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D315" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E315" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F315" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G315" s="4" t="s">
         <v>4</v>
@@ -4181,7 +4181,7 @@
     </row>
     <row r="316" spans="1:7">
       <c r="A316" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B316" s="5">
         <v>1</v>
@@ -4194,7 +4194,7 @@
     </row>
     <row r="317" spans="1:7">
       <c r="A317" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B317" s="8">
         <f>1/C316</f>
@@ -4210,7 +4210,7 @@
     </row>
     <row r="318" spans="1:7">
       <c r="A318" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B318" s="8">
         <f>1/D316</f>
@@ -4229,7 +4229,7 @@
     </row>
     <row r="319" spans="1:7">
       <c r="A319" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B319" s="8">
         <f>1/E316</f>
@@ -4251,7 +4251,7 @@
     </row>
     <row r="320" spans="1:7">
       <c r="A320" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B320" s="8">
         <f>1/F316</f>
@@ -4275,196 +4275,196 @@
       <c r="G320" s="7"/>
     </row>
     <row r="323" spans="1:7">
-      <c r="A323" s="1" t="s">
-        <v>17</v>
+      <c r="A323" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="324" spans="1:7">
-      <c r="A324" s="2" t="s">
-        <v>1</v>
+      <c r="A324" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B324" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C324" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D324" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E324" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F324" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G324" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="325" spans="1:7">
-      <c r="A325" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B325" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C325" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D325" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E325" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A325" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B325" s="5">
+        <v>1</v>
+      </c>
+      <c r="C325" s="6"/>
+      <c r="D325" s="6"/>
+      <c r="E325" s="6"/>
+      <c r="F325" s="6"/>
+      <c r="G325" s="7"/>
     </row>
     <row r="326" spans="1:7">
       <c r="A326" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B326" s="5">
-        <v>1</v>
-      </c>
-      <c r="C326" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="B326" s="8">
+        <f>1/C325</f>
+        <v>0</v>
+      </c>
+      <c r="C326" s="5">
+        <v>1</v>
+      </c>
       <c r="D326" s="6"/>
-      <c r="E326" s="7"/>
+      <c r="E326" s="6"/>
+      <c r="F326" s="6"/>
+      <c r="G326" s="7"/>
     </row>
     <row r="327" spans="1:7">
       <c r="A327" s="4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B327" s="8">
-        <f>1/C326</f>
-        <v>0</v>
-      </c>
-      <c r="C327" s="5">
-        <v>1</v>
-      </c>
-      <c r="D327" s="6"/>
-      <c r="E327" s="7"/>
+        <f>1/D325</f>
+        <v>0</v>
+      </c>
+      <c r="C327" s="8">
+        <f>1/D326</f>
+        <v>0</v>
+      </c>
+      <c r="D327" s="5">
+        <v>1</v>
+      </c>
+      <c r="E327" s="6"/>
+      <c r="F327" s="6"/>
+      <c r="G327" s="7"/>
     </row>
     <row r="328" spans="1:7">
       <c r="A328" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B328" s="8">
+        <f>1/E325</f>
+        <v>0</v>
+      </c>
+      <c r="C328" s="8">
+        <f>1/E326</f>
+        <v>0</v>
+      </c>
+      <c r="D328" s="8">
+        <f>1/E327</f>
+        <v>0</v>
+      </c>
+      <c r="E328" s="5">
+        <v>1</v>
+      </c>
+      <c r="F328" s="6"/>
+      <c r="G328" s="7"/>
+    </row>
+    <row r="329" spans="1:7">
+      <c r="A329" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B329" s="8">
+        <f>1/F325</f>
+        <v>0</v>
+      </c>
+      <c r="C329" s="8">
+        <f>1/F326</f>
+        <v>0</v>
+      </c>
+      <c r="D329" s="8">
+        <f>1/F327</f>
+        <v>0</v>
+      </c>
+      <c r="E329" s="8">
+        <f>1/F328</f>
+        <v>0</v>
+      </c>
+      <c r="F329" s="5">
+        <v>1</v>
+      </c>
+      <c r="G329" s="7"/>
+    </row>
+    <row r="332" spans="1:7">
+      <c r="A332" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7">
+      <c r="A333" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7">
+      <c r="A334" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B334" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C334" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D334" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B328" s="8">
-        <f>1/D326</f>
-        <v>0</v>
-      </c>
-      <c r="C328" s="8">
-        <f>1/D327</f>
-        <v>0</v>
-      </c>
-      <c r="D328" s="5">
-        <v>1</v>
-      </c>
-      <c r="E328" s="7"/>
-    </row>
-    <row r="331" spans="1:7">
-      <c r="A331" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="332" spans="1:7">
-      <c r="A332" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B332" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C332" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D332" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E332" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F332" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G332" s="4" t="s">
+      <c r="E334" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="333" spans="1:7">
-      <c r="A333" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B333" s="5">
-        <v>1</v>
-      </c>
-      <c r="C333" s="6"/>
-      <c r="D333" s="6"/>
-      <c r="E333" s="6"/>
-      <c r="F333" s="6"/>
-      <c r="G333" s="7"/>
-    </row>
-    <row r="334" spans="1:7">
-      <c r="A334" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B334" s="8">
-        <f>1/C333</f>
-        <v>0</v>
-      </c>
-      <c r="C334" s="5">
-        <v>1</v>
-      </c>
-      <c r="D334" s="6"/>
-      <c r="E334" s="6"/>
-      <c r="F334" s="6"/>
-      <c r="G334" s="7"/>
     </row>
     <row r="335" spans="1:7">
       <c r="A335" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B335" s="8">
-        <f>1/D333</f>
-        <v>0</v>
-      </c>
-      <c r="C335" s="8">
-        <f>1/D334</f>
-        <v>0</v>
-      </c>
-      <c r="D335" s="5">
-        <v>1</v>
-      </c>
-      <c r="E335" s="6"/>
-      <c r="F335" s="6"/>
-      <c r="G335" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="B335" s="5">
+        <v>1</v>
+      </c>
+      <c r="C335" s="6"/>
+      <c r="D335" s="6"/>
+      <c r="E335" s="7"/>
     </row>
     <row r="336" spans="1:7">
       <c r="A336" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B336" s="8">
-        <f>1/E333</f>
-        <v>0</v>
-      </c>
-      <c r="C336" s="8">
-        <f>1/E334</f>
-        <v>0</v>
-      </c>
-      <c r="D336" s="8">
-        <f>1/E335</f>
-        <v>0</v>
-      </c>
-      <c r="E336" s="5">
-        <v>1</v>
-      </c>
-      <c r="F336" s="6"/>
-      <c r="G336" s="7"/>
+        <f>1/C335</f>
+        <v>0</v>
+      </c>
+      <c r="C336" s="5">
+        <v>1</v>
+      </c>
+      <c r="D336" s="6"/>
+      <c r="E336" s="7"/>
     </row>
     <row r="337" spans="1:7">
       <c r="A337" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B337" s="8">
-        <f>1/F333</f>
+        <f>1/D335</f>
         <v>0</v>
       </c>
       <c r="C337" s="8">
-        <f>1/F334</f>
-        <v>0</v>
-      </c>
-      <c r="D337" s="8">
-        <f>1/F335</f>
-        <v>0</v>
-      </c>
-      <c r="E337" s="8">
-        <f>1/F336</f>
-        <v>0</v>
-      </c>
-      <c r="F337" s="5">
-        <v>1</v>
-      </c>
-      <c r="G337" s="7"/>
+        <f>1/D336</f>
+        <v>0</v>
+      </c>
+      <c r="D337" s="5">
+        <v>1</v>
+      </c>
+      <c r="E337" s="7"/>
     </row>
     <row r="340" spans="1:7">
       <c r="A340" s="2" t="s">
@@ -4473,27 +4473,30 @@
     </row>
     <row r="341" spans="1:7">
       <c r="A341" s="3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B341" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C341" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D341" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E341" s="4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F341" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G341" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="342" spans="1:7">
       <c r="A342" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B342" s="5">
         <v>1</v>
@@ -4501,11 +4504,12 @@
       <c r="C342" s="6"/>
       <c r="D342" s="6"/>
       <c r="E342" s="6"/>
-      <c r="F342" s="7"/>
+      <c r="F342" s="6"/>
+      <c r="G342" s="7"/>
     </row>
     <row r="343" spans="1:7">
       <c r="A343" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B343" s="8">
         <f>1/C342</f>
@@ -4516,11 +4520,12 @@
       </c>
       <c r="D343" s="6"/>
       <c r="E343" s="6"/>
-      <c r="F343" s="7"/>
+      <c r="F343" s="6"/>
+      <c r="G343" s="7"/>
     </row>
     <row r="344" spans="1:7">
       <c r="A344" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B344" s="8">
         <f>1/D342</f>
@@ -4534,11 +4539,12 @@
         <v>1</v>
       </c>
       <c r="E344" s="6"/>
-      <c r="F344" s="7"/>
+      <c r="F344" s="6"/>
+      <c r="G344" s="7"/>
     </row>
     <row r="345" spans="1:7">
       <c r="A345" s="4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B345" s="8">
         <f>1/E342</f>
@@ -4555,12 +4561,33 @@
       <c r="E345" s="5">
         <v>1</v>
       </c>
-      <c r="F345" s="7"/>
-    </row>
-    <row r="348" spans="1:7">
-      <c r="A348" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="F345" s="6"/>
+      <c r="G345" s="7"/>
+    </row>
+    <row r="346" spans="1:7">
+      <c r="A346" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B346" s="8">
+        <f>1/F342</f>
+        <v>0</v>
+      </c>
+      <c r="C346" s="8">
+        <f>1/F343</f>
+        <v>0</v>
+      </c>
+      <c r="D346" s="8">
+        <f>1/F344</f>
+        <v>0</v>
+      </c>
+      <c r="E346" s="8">
+        <f>1/F345</f>
+        <v>0</v>
+      </c>
+      <c r="F346" s="5">
+        <v>1</v>
+      </c>
+      <c r="G346" s="7"/>
     </row>
     <row r="349" spans="1:7">
       <c r="A349" s="2" t="s">
@@ -4569,35 +4596,39 @@
     </row>
     <row r="350" spans="1:7">
       <c r="A350" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B350" s="4" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C350" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D350" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E350" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F350" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="351" spans="1:7">
       <c r="A351" s="4" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B351" s="5">
         <v>1</v>
       </c>
       <c r="C351" s="6"/>
       <c r="D351" s="6"/>
-      <c r="E351" s="7"/>
+      <c r="E351" s="6"/>
+      <c r="F351" s="7"/>
     </row>
     <row r="352" spans="1:7">
       <c r="A352" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B352" s="8">
         <f>1/C351</f>
@@ -4607,11 +4638,12 @@
         <v>1</v>
       </c>
       <c r="D352" s="6"/>
-      <c r="E352" s="7"/>
+      <c r="E352" s="6"/>
+      <c r="F352" s="7"/>
     </row>
     <row r="353" spans="1:7">
       <c r="A353" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B353" s="8">
         <f>1/D351</f>
@@ -4624,130 +4656,98 @@
       <c r="D353" s="5">
         <v>1</v>
       </c>
-      <c r="E353" s="7"/>
-    </row>
-    <row r="356" spans="1:7">
-      <c r="A356" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="E353" s="6"/>
+      <c r="F353" s="7"/>
+    </row>
+    <row r="354" spans="1:7">
+      <c r="A354" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B354" s="8">
+        <f>1/E351</f>
+        <v>0</v>
+      </c>
+      <c r="C354" s="8">
+        <f>1/E352</f>
+        <v>0</v>
+      </c>
+      <c r="D354" s="8">
+        <f>1/E353</f>
+        <v>0</v>
+      </c>
+      <c r="E354" s="5">
+        <v>1</v>
+      </c>
+      <c r="F354" s="7"/>
     </row>
     <row r="357" spans="1:7">
-      <c r="A357" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B357" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C357" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D357" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E357" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F357" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G357" s="4" t="s">
+      <c r="A357" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7">
+      <c r="A358" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7">
+      <c r="A359" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B359" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C359" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D359" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E359" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="358" spans="1:7">
-      <c r="A358" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B358" s="5">
-        <v>1</v>
-      </c>
-      <c r="C358" s="6"/>
-      <c r="D358" s="6"/>
-      <c r="E358" s="6"/>
-      <c r="F358" s="6"/>
-      <c r="G358" s="7"/>
-    </row>
-    <row r="359" spans="1:7">
-      <c r="A359" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B359" s="8">
-        <f>1/C358</f>
-        <v>0</v>
-      </c>
-      <c r="C359" s="5">
-        <v>1</v>
-      </c>
-      <c r="D359" s="6"/>
-      <c r="E359" s="6"/>
-      <c r="F359" s="6"/>
-      <c r="G359" s="7"/>
     </row>
     <row r="360" spans="1:7">
       <c r="A360" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B360" s="8">
-        <f>1/D358</f>
-        <v>0</v>
-      </c>
-      <c r="C360" s="8">
-        <f>1/D359</f>
-        <v>0</v>
-      </c>
-      <c r="D360" s="5">
-        <v>1</v>
-      </c>
-      <c r="E360" s="6"/>
-      <c r="F360" s="6"/>
-      <c r="G360" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="B360" s="5">
+        <v>1</v>
+      </c>
+      <c r="C360" s="6"/>
+      <c r="D360" s="6"/>
+      <c r="E360" s="7"/>
     </row>
     <row r="361" spans="1:7">
       <c r="A361" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B361" s="8">
-        <f>1/E358</f>
-        <v>0</v>
-      </c>
-      <c r="C361" s="8">
-        <f>1/E359</f>
-        <v>0</v>
-      </c>
-      <c r="D361" s="8">
-        <f>1/E360</f>
-        <v>0</v>
-      </c>
-      <c r="E361" s="5">
-        <v>1</v>
-      </c>
-      <c r="F361" s="6"/>
-      <c r="G361" s="7"/>
+        <f>1/C360</f>
+        <v>0</v>
+      </c>
+      <c r="C361" s="5">
+        <v>1</v>
+      </c>
+      <c r="D361" s="6"/>
+      <c r="E361" s="7"/>
     </row>
     <row r="362" spans="1:7">
       <c r="A362" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B362" s="8">
-        <f>1/F358</f>
+        <f>1/D360</f>
         <v>0</v>
       </c>
       <c r="C362" s="8">
-        <f>1/F359</f>
-        <v>0</v>
-      </c>
-      <c r="D362" s="8">
-        <f>1/F360</f>
-        <v>0</v>
-      </c>
-      <c r="E362" s="8">
-        <f>1/F361</f>
-        <v>0</v>
-      </c>
-      <c r="F362" s="5">
-        <v>1</v>
-      </c>
-      <c r="G362" s="7"/>
+        <f>1/D361</f>
+        <v>0</v>
+      </c>
+      <c r="D362" s="5">
+        <v>1</v>
+      </c>
+      <c r="E362" s="7"/>
     </row>
     <row r="365" spans="1:7">
       <c r="A365" s="2" t="s">
@@ -4756,27 +4756,30 @@
     </row>
     <row r="366" spans="1:7">
       <c r="A366" s="3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B366" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C366" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D366" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E366" s="4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F366" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G366" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="367" spans="1:7">
       <c r="A367" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B367" s="5">
         <v>1</v>
@@ -4784,11 +4787,12 @@
       <c r="C367" s="6"/>
       <c r="D367" s="6"/>
       <c r="E367" s="6"/>
-      <c r="F367" s="7"/>
+      <c r="F367" s="6"/>
+      <c r="G367" s="7"/>
     </row>
     <row r="368" spans="1:7">
       <c r="A368" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B368" s="8">
         <f>1/C367</f>
@@ -4799,11 +4803,12 @@
       </c>
       <c r="D368" s="6"/>
       <c r="E368" s="6"/>
-      <c r="F368" s="7"/>
+      <c r="F368" s="6"/>
+      <c r="G368" s="7"/>
     </row>
     <row r="369" spans="1:7">
       <c r="A369" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B369" s="8">
         <f>1/D367</f>
@@ -4817,11 +4822,12 @@
         <v>1</v>
       </c>
       <c r="E369" s="6"/>
-      <c r="F369" s="7"/>
+      <c r="F369" s="6"/>
+      <c r="G369" s="7"/>
     </row>
     <row r="370" spans="1:7">
       <c r="A370" s="4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B370" s="8">
         <f>1/E367</f>
@@ -4838,12 +4844,33 @@
       <c r="E370" s="5">
         <v>1</v>
       </c>
-      <c r="F370" s="7"/>
-    </row>
-    <row r="373" spans="1:7">
-      <c r="A373" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="F370" s="6"/>
+      <c r="G370" s="7"/>
+    </row>
+    <row r="371" spans="1:7">
+      <c r="A371" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B371" s="8">
+        <f>1/F367</f>
+        <v>0</v>
+      </c>
+      <c r="C371" s="8">
+        <f>1/F368</f>
+        <v>0</v>
+      </c>
+      <c r="D371" s="8">
+        <f>1/F369</f>
+        <v>0</v>
+      </c>
+      <c r="E371" s="8">
+        <f>1/F370</f>
+        <v>0</v>
+      </c>
+      <c r="F371" s="5">
+        <v>1</v>
+      </c>
+      <c r="G371" s="7"/>
     </row>
     <row r="374" spans="1:7">
       <c r="A374" s="2" t="s">
@@ -4852,35 +4879,39 @@
     </row>
     <row r="375" spans="1:7">
       <c r="A375" s="3" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B375" s="4" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C375" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D375" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E375" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F375" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="376" spans="1:7">
       <c r="A376" s="4" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B376" s="5">
         <v>1</v>
       </c>
       <c r="C376" s="6"/>
       <c r="D376" s="6"/>
-      <c r="E376" s="7"/>
+      <c r="E376" s="6"/>
+      <c r="F376" s="7"/>
     </row>
     <row r="377" spans="1:7">
       <c r="A377" s="4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B377" s="8">
         <f>1/C376</f>
@@ -4890,11 +4921,12 @@
         <v>1</v>
       </c>
       <c r="D377" s="6"/>
-      <c r="E377" s="7"/>
+      <c r="E377" s="6"/>
+      <c r="F377" s="7"/>
     </row>
     <row r="378" spans="1:7">
       <c r="A378" s="4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B378" s="8">
         <f>1/D376</f>
@@ -4907,130 +4939,98 @@
       <c r="D378" s="5">
         <v>1</v>
       </c>
-      <c r="E378" s="7"/>
-    </row>
-    <row r="381" spans="1:7">
-      <c r="A381" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="E378" s="6"/>
+      <c r="F378" s="7"/>
+    </row>
+    <row r="379" spans="1:7">
+      <c r="A379" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B379" s="8">
+        <f>1/E376</f>
+        <v>0</v>
+      </c>
+      <c r="C379" s="8">
+        <f>1/E377</f>
+        <v>0</v>
+      </c>
+      <c r="D379" s="8">
+        <f>1/E378</f>
+        <v>0</v>
+      </c>
+      <c r="E379" s="5">
+        <v>1</v>
+      </c>
+      <c r="F379" s="7"/>
     </row>
     <row r="382" spans="1:7">
-      <c r="A382" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B382" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C382" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D382" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E382" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F382" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G382" s="4" t="s">
+      <c r="A382" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7">
+      <c r="A383" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7">
+      <c r="A384" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B384" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C384" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D384" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E384" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="383" spans="1:7">
-      <c r="A383" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B383" s="5">
-        <v>1</v>
-      </c>
-      <c r="C383" s="6"/>
-      <c r="D383" s="6"/>
-      <c r="E383" s="6"/>
-      <c r="F383" s="6"/>
-      <c r="G383" s="7"/>
-    </row>
-    <row r="384" spans="1:7">
-      <c r="A384" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B384" s="8">
-        <f>1/C383</f>
-        <v>0</v>
-      </c>
-      <c r="C384" s="5">
-        <v>1</v>
-      </c>
-      <c r="D384" s="6"/>
-      <c r="E384" s="6"/>
-      <c r="F384" s="6"/>
-      <c r="G384" s="7"/>
     </row>
     <row r="385" spans="1:7">
       <c r="A385" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B385" s="8">
-        <f>1/D383</f>
-        <v>0</v>
-      </c>
-      <c r="C385" s="8">
-        <f>1/D384</f>
-        <v>0</v>
-      </c>
-      <c r="D385" s="5">
-        <v>1</v>
-      </c>
-      <c r="E385" s="6"/>
-      <c r="F385" s="6"/>
-      <c r="G385" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="B385" s="5">
+        <v>1</v>
+      </c>
+      <c r="C385" s="6"/>
+      <c r="D385" s="6"/>
+      <c r="E385" s="7"/>
     </row>
     <row r="386" spans="1:7">
       <c r="A386" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B386" s="8">
-        <f>1/E383</f>
-        <v>0</v>
-      </c>
-      <c r="C386" s="8">
-        <f>1/E384</f>
-        <v>0</v>
-      </c>
-      <c r="D386" s="8">
-        <f>1/E385</f>
-        <v>0</v>
-      </c>
-      <c r="E386" s="5">
-        <v>1</v>
-      </c>
-      <c r="F386" s="6"/>
-      <c r="G386" s="7"/>
+        <f>1/C385</f>
+        <v>0</v>
+      </c>
+      <c r="C386" s="5">
+        <v>1</v>
+      </c>
+      <c r="D386" s="6"/>
+      <c r="E386" s="7"/>
     </row>
     <row r="387" spans="1:7">
       <c r="A387" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B387" s="8">
-        <f>1/F383</f>
+        <f>1/D385</f>
         <v>0</v>
       </c>
       <c r="C387" s="8">
-        <f>1/F384</f>
-        <v>0</v>
-      </c>
-      <c r="D387" s="8">
-        <f>1/F385</f>
-        <v>0</v>
-      </c>
-      <c r="E387" s="8">
-        <f>1/F386</f>
-        <v>0</v>
-      </c>
-      <c r="F387" s="5">
-        <v>1</v>
-      </c>
-      <c r="G387" s="7"/>
+        <f>1/D386</f>
+        <v>0</v>
+      </c>
+      <c r="D387" s="5">
+        <v>1</v>
+      </c>
+      <c r="E387" s="7"/>
     </row>
     <row r="390" spans="1:7">
       <c r="A390" s="2" t="s">
@@ -5039,22 +5039,22 @@
     </row>
     <row r="391" spans="1:7">
       <c r="A391" s="3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B391" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C391" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D391" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E391" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F391" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G391" s="4" t="s">
         <v>4</v>
@@ -5062,7 +5062,7 @@
     </row>
     <row r="392" spans="1:7">
       <c r="A392" s="4" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B392" s="5">
         <v>1</v>
@@ -5075,7 +5075,7 @@
     </row>
     <row r="393" spans="1:7">
       <c r="A393" s="4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B393" s="8">
         <f>1/C392</f>
@@ -5091,7 +5091,7 @@
     </row>
     <row r="394" spans="1:7">
       <c r="A394" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B394" s="8">
         <f>1/D392</f>
@@ -5110,7 +5110,7 @@
     </row>
     <row r="395" spans="1:7">
       <c r="A395" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B395" s="8">
         <f>1/E392</f>
@@ -5132,7 +5132,7 @@
     </row>
     <row r="396" spans="1:7">
       <c r="A396" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B396" s="8">
         <f>1/F392</f>
@@ -5156,233 +5156,241 @@
       <c r="G396" s="7"/>
     </row>
     <row r="399" spans="1:7">
-      <c r="A399" s="1" t="s">
-        <v>20</v>
+      <c r="A399" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="400" spans="1:7">
-      <c r="A400" s="2" t="s">
-        <v>1</v>
+      <c r="A400" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B400" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C400" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D400" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E400" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F400" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G400" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="401" spans="1:7">
-      <c r="A401" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B401" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C401" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D401" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E401" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A401" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B401" s="5">
+        <v>1</v>
+      </c>
+      <c r="C401" s="6"/>
+      <c r="D401" s="6"/>
+      <c r="E401" s="6"/>
+      <c r="F401" s="6"/>
+      <c r="G401" s="7"/>
     </row>
     <row r="402" spans="1:7">
       <c r="A402" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B402" s="5">
-        <v>1</v>
-      </c>
-      <c r="C402" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="B402" s="8">
+        <f>1/C401</f>
+        <v>0</v>
+      </c>
+      <c r="C402" s="5">
+        <v>1</v>
+      </c>
       <c r="D402" s="6"/>
-      <c r="E402" s="7"/>
+      <c r="E402" s="6"/>
+      <c r="F402" s="6"/>
+      <c r="G402" s="7"/>
     </row>
     <row r="403" spans="1:7">
       <c r="A403" s="4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B403" s="8">
-        <f>1/C402</f>
-        <v>0</v>
-      </c>
-      <c r="C403" s="5">
-        <v>1</v>
-      </c>
-      <c r="D403" s="6"/>
-      <c r="E403" s="7"/>
+        <f>1/D401</f>
+        <v>0</v>
+      </c>
+      <c r="C403" s="8">
+        <f>1/D402</f>
+        <v>0</v>
+      </c>
+      <c r="D403" s="5">
+        <v>1</v>
+      </c>
+      <c r="E403" s="6"/>
+      <c r="F403" s="6"/>
+      <c r="G403" s="7"/>
     </row>
     <row r="404" spans="1:7">
       <c r="A404" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B404" s="8">
+        <f>1/E401</f>
+        <v>0</v>
+      </c>
+      <c r="C404" s="8">
+        <f>1/E402</f>
+        <v>0</v>
+      </c>
+      <c r="D404" s="8">
+        <f>1/E403</f>
+        <v>0</v>
+      </c>
+      <c r="E404" s="5">
+        <v>1</v>
+      </c>
+      <c r="F404" s="6"/>
+      <c r="G404" s="7"/>
+    </row>
+    <row r="405" spans="1:7">
+      <c r="A405" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B405" s="8">
+        <f>1/F401</f>
+        <v>0</v>
+      </c>
+      <c r="C405" s="8">
+        <f>1/F402</f>
+        <v>0</v>
+      </c>
+      <c r="D405" s="8">
+        <f>1/F403</f>
+        <v>0</v>
+      </c>
+      <c r="E405" s="8">
+        <f>1/F404</f>
+        <v>0</v>
+      </c>
+      <c r="F405" s="5">
+        <v>1</v>
+      </c>
+      <c r="G405" s="7"/>
+    </row>
+    <row r="408" spans="1:7">
+      <c r="A408" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="409" spans="1:7">
+      <c r="A409" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="410" spans="1:7">
+      <c r="A410" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B410" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C410" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D410" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B404" s="8">
-        <f>1/D402</f>
-        <v>0</v>
-      </c>
-      <c r="C404" s="8">
-        <f>1/D403</f>
-        <v>0</v>
-      </c>
-      <c r="D404" s="5">
-        <v>1</v>
-      </c>
-      <c r="E404" s="7"/>
-    </row>
-    <row r="407" spans="1:7">
-      <c r="A407" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="408" spans="1:7">
-      <c r="A408" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B408" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C408" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D408" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E408" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F408" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G408" s="4" t="s">
+      <c r="E410" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="409" spans="1:7">
-      <c r="A409" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B409" s="5">
-        <v>1</v>
-      </c>
-      <c r="C409" s="6"/>
-      <c r="D409" s="6"/>
-      <c r="E409" s="6"/>
-      <c r="F409" s="6"/>
-      <c r="G409" s="7"/>
-    </row>
-    <row r="410" spans="1:7">
-      <c r="A410" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B410" s="8">
-        <f>1/C409</f>
-        <v>0</v>
-      </c>
-      <c r="C410" s="5">
-        <v>1</v>
-      </c>
-      <c r="D410" s="6"/>
-      <c r="E410" s="6"/>
-      <c r="F410" s="6"/>
-      <c r="G410" s="7"/>
     </row>
     <row r="411" spans="1:7">
       <c r="A411" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B411" s="8">
-        <f>1/D409</f>
-        <v>0</v>
-      </c>
-      <c r="C411" s="8">
-        <f>1/D410</f>
-        <v>0</v>
-      </c>
-      <c r="D411" s="5">
-        <v>1</v>
-      </c>
-      <c r="E411" s="6"/>
-      <c r="F411" s="6"/>
-      <c r="G411" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="B411" s="5">
+        <v>1</v>
+      </c>
+      <c r="C411" s="6"/>
+      <c r="D411" s="6"/>
+      <c r="E411" s="7"/>
     </row>
     <row r="412" spans="1:7">
       <c r="A412" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B412" s="8">
-        <f>1/E409</f>
-        <v>0</v>
-      </c>
-      <c r="C412" s="8">
-        <f>1/E410</f>
-        <v>0</v>
-      </c>
-      <c r="D412" s="8">
-        <f>1/E411</f>
-        <v>0</v>
-      </c>
-      <c r="E412" s="5">
-        <v>1</v>
-      </c>
-      <c r="F412" s="6"/>
-      <c r="G412" s="7"/>
+        <f>1/C411</f>
+        <v>0</v>
+      </c>
+      <c r="C412" s="5">
+        <v>1</v>
+      </c>
+      <c r="D412" s="6"/>
+      <c r="E412" s="7"/>
     </row>
     <row r="413" spans="1:7">
       <c r="A413" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B413" s="8">
-        <f>1/F409</f>
+        <f>1/D411</f>
         <v>0</v>
       </c>
       <c r="C413" s="8">
-        <f>1/F410</f>
-        <v>0</v>
-      </c>
-      <c r="D413" s="8">
-        <f>1/F411</f>
-        <v>0</v>
-      </c>
-      <c r="E413" s="8">
-        <f>1/F412</f>
-        <v>0</v>
-      </c>
-      <c r="F413" s="5">
-        <v>1</v>
-      </c>
-      <c r="G413" s="7"/>
+        <f>1/D412</f>
+        <v>0</v>
+      </c>
+      <c r="D413" s="5">
+        <v>1</v>
+      </c>
+      <c r="E413" s="7"/>
     </row>
     <row r="416" spans="1:7">
       <c r="A416" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="417" spans="1:5">
+    <row r="417" spans="1:7">
       <c r="A417" s="3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B417" s="4" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C417" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D417" s="4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E417" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F417" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G417" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="418" spans="1:5">
+    <row r="418" spans="1:7">
       <c r="A418" s="4" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B418" s="5">
         <v>1</v>
       </c>
       <c r="C418" s="6"/>
       <c r="D418" s="6"/>
-      <c r="E418" s="7"/>
-    </row>
-    <row r="419" spans="1:5">
+      <c r="E418" s="6"/>
+      <c r="F418" s="6"/>
+      <c r="G418" s="7"/>
+    </row>
+    <row r="419" spans="1:7">
       <c r="A419" s="4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B419" s="8">
         <f>1/C418</f>
@@ -5392,11 +5400,13 @@
         <v>1</v>
       </c>
       <c r="D419" s="6"/>
-      <c r="E419" s="7"/>
-    </row>
-    <row r="420" spans="1:5">
+      <c r="E419" s="6"/>
+      <c r="F419" s="6"/>
+      <c r="G419" s="7"/>
+    </row>
+    <row r="420" spans="1:7">
       <c r="A420" s="4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B420" s="8">
         <f>1/D418</f>
@@ -5409,7 +5419,120 @@
       <c r="D420" s="5">
         <v>1</v>
       </c>
-      <c r="E420" s="7"/>
+      <c r="E420" s="6"/>
+      <c r="F420" s="6"/>
+      <c r="G420" s="7"/>
+    </row>
+    <row r="421" spans="1:7">
+      <c r="A421" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B421" s="8">
+        <f>1/E418</f>
+        <v>0</v>
+      </c>
+      <c r="C421" s="8">
+        <f>1/E419</f>
+        <v>0</v>
+      </c>
+      <c r="D421" s="8">
+        <f>1/E420</f>
+        <v>0</v>
+      </c>
+      <c r="E421" s="5">
+        <v>1</v>
+      </c>
+      <c r="F421" s="6"/>
+      <c r="G421" s="7"/>
+    </row>
+    <row r="422" spans="1:7">
+      <c r="A422" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B422" s="8">
+        <f>1/F418</f>
+        <v>0</v>
+      </c>
+      <c r="C422" s="8">
+        <f>1/F419</f>
+        <v>0</v>
+      </c>
+      <c r="D422" s="8">
+        <f>1/F420</f>
+        <v>0</v>
+      </c>
+      <c r="E422" s="8">
+        <f>1/F421</f>
+        <v>0</v>
+      </c>
+      <c r="F422" s="5">
+        <v>1</v>
+      </c>
+      <c r="G422" s="7"/>
+    </row>
+    <row r="425" spans="1:7">
+      <c r="A425" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="426" spans="1:7">
+      <c r="A426" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B426" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C426" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D426" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E426" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="427" spans="1:7">
+      <c r="A427" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B427" s="5">
+        <v>1</v>
+      </c>
+      <c r="C427" s="6"/>
+      <c r="D427" s="6"/>
+      <c r="E427" s="7"/>
+    </row>
+    <row r="428" spans="1:7">
+      <c r="A428" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B428" s="8">
+        <f>1/C427</f>
+        <v>0</v>
+      </c>
+      <c r="C428" s="5">
+        <v>1</v>
+      </c>
+      <c r="D428" s="6"/>
+      <c r="E428" s="7"/>
+    </row>
+    <row r="429" spans="1:7">
+      <c r="A429" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B429" s="8">
+        <f>1/D427</f>
+        <v>0</v>
+      </c>
+      <c r="C429" s="8">
+        <f>1/D428</f>
+        <v>0</v>
+      </c>
+      <c r="D429" s="5">
+        <v>1</v>
+      </c>
+      <c r="E429" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>